<commit_message>
add some tests related to fdo#42624
see fdo#44587 for problems with range names in matrix formulas during xlsx
import/export
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/named-ranges-global.xlsx
+++ b/sc/qa/unit/data/xlsx/named-ranges-global.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="254" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="667" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" name="Global1" vbProcedure="false">Sheet1!$A$1</definedName>
     <definedName function="false" hidden="false" name="Global2" vbProcedure="false">Sheet1!$A$2</definedName>
     <definedName function="false" hidden="false" name="Global3" vbProcedure="false">Sheet1!$A$1:$A$4</definedName>
+    <definedName function="false" hidden="false" name="Global4" vbProcedure="false">{1,2,3;4,5,6}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Local1" vbProcedure="false">Sheet1!$A$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Local2" vbProcedure="false">Sheet1!$A$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Local1" vbProcedure="false">Sheet1!$A$5</definedName>
@@ -32,6 +33,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -115,14 +117,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A4:C5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>1</v>
       </c>
@@ -135,7 +138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
@@ -144,7 +147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
@@ -153,7 +156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>4</v>
       </c>
@@ -162,7 +165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>5</v>
       </c>
@@ -183,14 +186,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A4:C5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -211,10 +215,38 @@
         <v>7</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <f aca="false">Global4</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
add test for range name import, related fdo#42624
this adds range names referencing range names that are loaded after the
referencing range name
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/named-ranges-global.xlsx
+++ b/sc/qa/unit/data/xlsx/named-ranges-global.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="667" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="483" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,8 @@
     <definedName function="false" hidden="false" name="Global2" vbProcedure="false">Sheet1!$A$2</definedName>
     <definedName function="false" hidden="false" name="Global3" vbProcedure="false">Sheet1!$A$1:$A$4</definedName>
     <definedName function="false" hidden="false" name="Global4" vbProcedure="false">{1,2,3;4,5,6}</definedName>
+    <definedName function="false" hidden="false" name="Global5" vbProcedure="false">Global6</definedName>
+    <definedName function="false" hidden="false" name="Global6" vbProcedure="false">Sheet2!$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Local1" vbProcedure="false">Sheet1!$A$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Local2" vbProcedure="false">Sheet1!$A$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Local1" vbProcedure="false">Sheet1!$A$5</definedName>
@@ -33,7 +35,6 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -117,15 +118,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A4:C5"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>1</v>
       </c>
@@ -138,7 +139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
@@ -147,7 +148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
@@ -156,7 +157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>4</v>
       </c>
@@ -165,7 +166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>5</v>
       </c>
@@ -186,15 +187,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A4:C5"/>
+      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -243,10 +244,16 @@
         <v>6</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="n">
+        <f aca="false">Global5</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
unit test for bnc#780296 fix
Change-Id: Ib75437bb52c8094821fc9d18429f4ce01bb7ec2f
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/named-ranges-global.xlsx
+++ b/sc/qa/unit/data/xlsx/named-ranges-global.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="483" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
@@ -16,7 +16,7 @@
     <definedName function="false" hidden="false" name="Global2" vbProcedure="false">Sheet1!$A$2</definedName>
     <definedName function="false" hidden="false" name="Global3" vbProcedure="false">Sheet1!$A$1:$A$4</definedName>
     <definedName function="false" hidden="false" name="Global4" vbProcedure="false">{1,2,3;4,5,6}</definedName>
-    <definedName function="false" hidden="false" name="Global5" vbProcedure="false">Global6</definedName>
+    <definedName function="false" hidden="false" name="Global5" vbProcedure="false">global6</definedName>
     <definedName function="false" hidden="false" name="Global6" vbProcedure="false">Sheet2!$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Local1" vbProcedure="false">Sheet1!$A$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Local2" vbProcedure="false">Sheet1!$A$4</definedName>
@@ -35,6 +35,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -118,15 +119,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.9019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.55" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>1</v>
       </c>
@@ -139,7 +140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.55" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
@@ -148,7 +149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.55" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
@@ -157,7 +158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.55" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>4</v>
       </c>
@@ -166,7 +167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.55" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>5</v>
       </c>
@@ -187,18 +188,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
+      <selection activeCell="C7" activeCellId="0" pane="topLeft" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.9019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>6</v>
       </c>
@@ -207,7 +208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>7</v>
       </c>
@@ -216,7 +217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <f aca="false">Global4</f>
         <v>1</v>
@@ -230,7 +231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <f aca="false">A4</f>
         <v>4</v>
@@ -244,16 +245,17 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="e">
         <f aca="false">Global5</f>
-        <v>5</v>
-      </c>
-    </row>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>